<commit_message>
creating csv from external_choices + better errors
</commit_message>
<xml_diff>
--- a/pyxform/tests/example_xls/select_one_external.xlsx
+++ b/pyxform/tests/example_xls/select_one_external.xlsx
@@ -5,7 +5,8 @@
   <sheets>
     <sheet sheetId="1" name="survey" state="visible" r:id="rId3"/>
     <sheet sheetId="2" name="choices" state="visible" r:id="rId4"/>
-    <sheet sheetId="3" name="settings" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="external_choices" state="visible" r:id="rId5"/>
+    <sheet sheetId="4" name="settings" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -27,7 +28,7 @@
     <t>choice_filter</t>
   </si>
   <si>
-    <t>select_one_external states</t>
+    <t>select_one states</t>
   </si>
   <si>
     <t>state</t>
@@ -69,6 +70,33 @@
     <t>label</t>
   </si>
   <si>
+    <t>states</t>
+  </si>
+  <si>
+    <t>texas</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>states</t>
+  </si>
+  <si>
+    <t>washington</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
     <t>state</t>
   </si>
   <si>
@@ -256,6 +284,9 @@
   </si>
   <si>
     <t>washington</t>
+  </si>
+  <si>
+    <t>no column header test</t>
   </si>
   <si>
     <t>pierce</t>
@@ -277,7 +308,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <name val="Arial"/>
@@ -301,6 +332,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -331,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf fillId="0" numFmtId="0" borderId="0" fontId="0"/>
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="1">
       <alignment vertical="center"/>
@@ -344,6 +376,9 @@
     </xf>
     <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="4">
       <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" fillId="2" xfId="0" numFmtId="0" borderId="1" applyFont="1" fontId="5">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -363,6 +398,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -772,12 +811,8 @@
       <c t="s" s="1" r="C1">
         <v>17</v>
       </c>
-      <c t="s" s="1" r="D1">
-        <v>18</v>
-      </c>
-      <c t="s" s="1" r="E1">
-        <v>19</v>
-      </c>
+      <c s="1" r="D1"/>
+      <c s="1" r="E1"/>
       <c s="3" r="F1"/>
       <c s="3" r="G1"/>
       <c s="3" r="H1"/>
@@ -791,13 +826,13 @@
     </row>
     <row customHeight="1" r="2" ht="14.25">
       <c t="s" s="1" r="A2">
+        <v>18</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>19</v>
+      </c>
+      <c t="s" s="1" r="C2">
         <v>20</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="C2">
-        <v>22</v>
       </c>
       <c s="3" r="D2"/>
       <c s="3" r="E2"/>
@@ -814,13 +849,13 @@
     </row>
     <row customHeight="1" r="3" ht="14.25">
       <c t="s" s="1" r="A3">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>22</v>
+      </c>
+      <c t="s" s="1" r="C3">
         <v>23</v>
-      </c>
-      <c t="s" s="1" r="B3">
-        <v>24</v>
-      </c>
-      <c t="s" s="1" r="C3">
-        <v>25</v>
       </c>
       <c s="3" r="D3"/>
       <c s="3" r="E3"/>
@@ -836,18 +871,10 @@
       <c s="3" r="O3"/>
     </row>
     <row customHeight="1" r="4" ht="14.25">
-      <c t="s" s="1" r="A4">
-        <v>26</v>
-      </c>
-      <c t="s" s="1" r="B4">
-        <v>27</v>
-      </c>
-      <c t="s" s="1" r="C4">
-        <v>28</v>
-      </c>
-      <c t="s" s="1" r="D4">
-        <v>29</v>
-      </c>
+      <c s="1" r="A4"/>
+      <c s="1" r="B4"/>
+      <c s="1" r="C4"/>
+      <c s="1" r="D4"/>
       <c s="3" r="E4"/>
       <c s="3" r="F4"/>
       <c s="3" r="G4"/>
@@ -861,18 +888,10 @@
       <c s="3" r="O4"/>
     </row>
     <row customHeight="1" r="5" ht="14.25">
-      <c t="s" s="1" r="A5">
-        <v>30</v>
-      </c>
-      <c t="s" s="1" r="B5">
-        <v>31</v>
-      </c>
-      <c t="s" s="1" r="C5">
-        <v>32</v>
-      </c>
-      <c t="s" s="1" r="D5">
-        <v>33</v>
-      </c>
+      <c s="1" r="A5"/>
+      <c s="1" r="B5"/>
+      <c s="1" r="C5"/>
+      <c s="1" r="D5"/>
       <c s="3" r="E5"/>
       <c s="3" r="F5"/>
       <c s="3" r="G5"/>
@@ -886,18 +905,10 @@
       <c s="3" r="O5"/>
     </row>
     <row customHeight="1" r="6" ht="14.25">
-      <c t="s" s="1" r="A6">
-        <v>34</v>
-      </c>
-      <c t="s" s="1" r="B6">
-        <v>35</v>
-      </c>
-      <c t="s" s="1" r="C6">
-        <v>36</v>
-      </c>
-      <c t="s" s="1" r="D6">
-        <v>37</v>
-      </c>
+      <c s="1" r="A6"/>
+      <c s="1" r="B6"/>
+      <c s="1" r="C6"/>
+      <c s="1" r="D6"/>
       <c s="3" r="E6"/>
       <c s="3" r="F6"/>
       <c s="3" r="G6"/>
@@ -911,18 +922,10 @@
       <c s="3" r="O6"/>
     </row>
     <row customHeight="1" r="7" ht="14.25">
-      <c t="s" s="1" r="A7">
-        <v>38</v>
-      </c>
-      <c t="s" s="1" r="B7">
-        <v>39</v>
-      </c>
-      <c t="s" s="1" r="C7">
-        <v>40</v>
-      </c>
-      <c t="s" s="1" r="D7">
-        <v>41</v>
-      </c>
+      <c s="1" r="A7"/>
+      <c s="1" r="B7"/>
+      <c s="1" r="C7"/>
+      <c s="1" r="D7"/>
       <c s="3" r="E7"/>
       <c s="3" r="F7"/>
       <c s="3" r="G7"/>
@@ -936,21 +939,11 @@
       <c s="3" r="O7"/>
     </row>
     <row customHeight="1" r="8" ht="14.25">
-      <c t="s" s="1" r="A8">
-        <v>42</v>
-      </c>
-      <c t="s" s="1" r="B8">
-        <v>43</v>
-      </c>
-      <c t="s" s="1" r="C8">
-        <v>44</v>
-      </c>
-      <c t="s" s="1" r="D8">
-        <v>45</v>
-      </c>
-      <c t="s" s="1" r="E8">
-        <v>46</v>
-      </c>
+      <c s="1" r="A8"/>
+      <c s="1" r="B8"/>
+      <c s="1" r="C8"/>
+      <c s="1" r="D8"/>
+      <c s="1" r="E8"/>
       <c s="3" r="F8"/>
       <c s="3" r="G8"/>
       <c s="3" r="H8"/>
@@ -963,21 +956,11 @@
       <c s="3" r="O8"/>
     </row>
     <row customHeight="1" r="9" ht="14.25">
-      <c t="s" s="1" r="A9">
-        <v>47</v>
-      </c>
-      <c t="s" s="1" r="B9">
-        <v>48</v>
-      </c>
-      <c t="s" s="1" r="C9">
-        <v>49</v>
-      </c>
-      <c t="s" s="1" r="D9">
-        <v>50</v>
-      </c>
-      <c t="s" s="1" r="E9">
-        <v>51</v>
-      </c>
+      <c s="1" r="A9"/>
+      <c s="1" r="B9"/>
+      <c s="1" r="C9"/>
+      <c s="1" r="D9"/>
+      <c s="1" r="E9"/>
       <c s="3" r="F9"/>
       <c s="3" r="G9"/>
       <c s="3" r="H9"/>
@@ -990,21 +973,11 @@
       <c s="3" r="O9"/>
     </row>
     <row customHeight="1" r="10" ht="14.25">
-      <c t="s" s="1" r="A10">
-        <v>52</v>
-      </c>
-      <c t="s" s="1" r="B10">
-        <v>53</v>
-      </c>
-      <c t="s" s="1" r="C10">
-        <v>54</v>
-      </c>
-      <c t="s" s="1" r="D10">
-        <v>55</v>
-      </c>
-      <c t="s" s="1" r="E10">
-        <v>56</v>
-      </c>
+      <c s="1" r="A10"/>
+      <c s="1" r="B10"/>
+      <c s="1" r="C10"/>
+      <c s="1" r="D10"/>
+      <c s="1" r="E10"/>
       <c s="3" r="F10"/>
       <c s="3" r="G10"/>
       <c s="3" r="H10"/>
@@ -1017,21 +990,11 @@
       <c s="3" r="O10"/>
     </row>
     <row customHeight="1" r="11" ht="14.25">
-      <c t="s" s="1" r="A11">
-        <v>57</v>
-      </c>
-      <c t="s" s="1" r="B11">
-        <v>58</v>
-      </c>
-      <c t="s" s="1" r="C11">
-        <v>59</v>
-      </c>
-      <c t="s" s="1" r="D11">
-        <v>60</v>
-      </c>
-      <c t="s" s="1" r="E11">
-        <v>61</v>
-      </c>
+      <c s="1" r="A11"/>
+      <c s="1" r="B11"/>
+      <c s="1" r="C11"/>
+      <c s="1" r="D11"/>
+      <c s="1" r="E11"/>
       <c s="3" r="F11"/>
       <c s="3" r="G11"/>
       <c s="3" r="H11"/>
@@ -1044,21 +1007,11 @@
       <c s="3" r="O11"/>
     </row>
     <row customHeight="1" r="12" ht="14.25">
-      <c t="s" s="1" r="A12">
-        <v>62</v>
-      </c>
-      <c t="s" s="1" r="B12">
-        <v>63</v>
-      </c>
-      <c t="s" s="1" r="C12">
-        <v>64</v>
-      </c>
-      <c t="s" s="1" r="D12">
-        <v>65</v>
-      </c>
-      <c t="s" s="1" r="E12">
-        <v>66</v>
-      </c>
+      <c s="1" r="A12"/>
+      <c s="1" r="B12"/>
+      <c s="1" r="C12"/>
+      <c s="1" r="D12"/>
+      <c s="1" r="E12"/>
       <c s="3" r="F12"/>
       <c s="3" r="G12"/>
       <c s="3" r="H12"/>
@@ -1071,21 +1024,11 @@
       <c s="3" r="O12"/>
     </row>
     <row customHeight="1" r="13" ht="14.25">
-      <c t="s" s="1" r="A13">
-        <v>67</v>
-      </c>
-      <c t="s" s="1" r="B13">
-        <v>68</v>
-      </c>
-      <c t="s" s="1" r="C13">
-        <v>69</v>
-      </c>
-      <c t="s" s="1" r="D13">
-        <v>70</v>
-      </c>
-      <c t="s" s="1" r="E13">
-        <v>71</v>
-      </c>
+      <c s="1" r="A13"/>
+      <c s="1" r="B13"/>
+      <c s="1" r="C13"/>
+      <c s="1" r="D13"/>
+      <c s="1" r="E13"/>
       <c s="3" r="F13"/>
       <c s="3" r="G13"/>
       <c s="3" r="H13"/>
@@ -1098,21 +1041,11 @@
       <c s="3" r="O13"/>
     </row>
     <row customHeight="1" r="14" ht="14.25">
-      <c t="s" s="1" r="A14">
-        <v>72</v>
-      </c>
-      <c t="s" s="1" r="B14">
-        <v>73</v>
-      </c>
-      <c t="s" s="1" r="C14">
-        <v>74</v>
-      </c>
-      <c t="s" s="1" r="D14">
-        <v>75</v>
-      </c>
-      <c t="s" s="1" r="E14">
-        <v>76</v>
-      </c>
+      <c s="1" r="A14"/>
+      <c s="1" r="B14"/>
+      <c s="1" r="C14"/>
+      <c s="1" r="D14"/>
+      <c s="1" r="E14"/>
       <c s="3" r="F14"/>
       <c s="3" r="G14"/>
       <c s="3" r="H14"/>
@@ -1125,21 +1058,11 @@
       <c s="3" r="O14"/>
     </row>
     <row customHeight="1" r="15" ht="14.25">
-      <c t="s" s="1" r="A15">
-        <v>77</v>
-      </c>
-      <c t="s" s="1" r="B15">
-        <v>78</v>
-      </c>
-      <c t="s" s="1" r="C15">
-        <v>79</v>
-      </c>
-      <c t="s" s="1" r="D15">
-        <v>80</v>
-      </c>
-      <c t="s" s="1" r="E15">
-        <v>81</v>
-      </c>
+      <c s="1" r="A15"/>
+      <c s="1" r="B15"/>
+      <c s="1" r="C15"/>
+      <c s="1" r="D15"/>
+      <c s="1" r="E15"/>
       <c s="3" r="F15"/>
       <c s="3" r="G15"/>
       <c s="3" r="H15"/>
@@ -1247,6 +1170,260 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c t="s" s="1" r="A1">
+        <v>24</v>
+      </c>
+      <c t="s" s="1" r="B1">
+        <v>25</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>26</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>27</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2">
+      <c t="s" s="1" r="A2">
+        <v>29</v>
+      </c>
+      <c t="s" s="1" r="B2">
+        <v>30</v>
+      </c>
+      <c t="s" s="1" r="C2">
+        <v>31</v>
+      </c>
+      <c s="3" r="D2"/>
+      <c s="3" r="F2"/>
+    </row>
+    <row r="3">
+      <c t="s" s="1" r="A3">
+        <v>32</v>
+      </c>
+      <c t="s" s="1" r="B3">
+        <v>33</v>
+      </c>
+      <c t="s" s="1" r="C3">
+        <v>34</v>
+      </c>
+      <c s="3" r="D3"/>
+      <c s="3" r="F3"/>
+    </row>
+    <row r="4">
+      <c t="s" s="1" r="A4">
+        <v>35</v>
+      </c>
+      <c t="s" s="1" r="B4">
+        <v>36</v>
+      </c>
+      <c t="s" s="1" r="C4">
+        <v>37</v>
+      </c>
+      <c t="s" s="1" r="D4">
+        <v>38</v>
+      </c>
+      <c s="3" r="F4"/>
+    </row>
+    <row r="5">
+      <c t="s" s="1" r="A5">
+        <v>39</v>
+      </c>
+      <c t="s" s="1" r="B5">
+        <v>40</v>
+      </c>
+      <c t="s" s="1" r="C5">
+        <v>41</v>
+      </c>
+      <c t="s" s="1" r="D5">
+        <v>42</v>
+      </c>
+      <c s="3" r="F5"/>
+    </row>
+    <row r="6">
+      <c t="s" s="1" r="A6">
+        <v>43</v>
+      </c>
+      <c t="s" s="1" r="B6">
+        <v>44</v>
+      </c>
+      <c t="s" s="1" r="C6">
+        <v>45</v>
+      </c>
+      <c t="s" s="1" r="D6">
+        <v>46</v>
+      </c>
+      <c s="3" r="F6"/>
+    </row>
+    <row r="7">
+      <c t="s" s="1" r="A7">
+        <v>47</v>
+      </c>
+      <c t="s" s="1" r="B7">
+        <v>48</v>
+      </c>
+      <c t="s" s="1" r="C7">
+        <v>49</v>
+      </c>
+      <c t="s" s="1" r="D7">
+        <v>50</v>
+      </c>
+      <c s="3" r="F7"/>
+    </row>
+    <row r="8">
+      <c t="s" s="1" r="A8">
+        <v>51</v>
+      </c>
+      <c t="s" s="1" r="B8">
+        <v>52</v>
+      </c>
+      <c t="s" s="1" r="C8">
+        <v>53</v>
+      </c>
+      <c t="s" s="1" r="D8">
+        <v>54</v>
+      </c>
+      <c t="s" s="1" r="F8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c t="s" s="1" r="A9">
+        <v>56</v>
+      </c>
+      <c t="s" s="1" r="B9">
+        <v>57</v>
+      </c>
+      <c t="s" s="1" r="C9">
+        <v>58</v>
+      </c>
+      <c t="s" s="1" r="D9">
+        <v>59</v>
+      </c>
+      <c t="s" s="1" r="F9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10">
+      <c t="s" s="1" r="A10">
+        <v>61</v>
+      </c>
+      <c t="s" s="1" r="B10">
+        <v>62</v>
+      </c>
+      <c t="s" s="1" r="C10">
+        <v>63</v>
+      </c>
+      <c t="s" s="1" r="D10">
+        <v>64</v>
+      </c>
+      <c t="s" s="1" r="F10">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11">
+      <c t="s" s="1" r="A11">
+        <v>66</v>
+      </c>
+      <c t="s" s="1" r="B11">
+        <v>67</v>
+      </c>
+      <c t="s" s="1" r="C11">
+        <v>68</v>
+      </c>
+      <c t="s" s="1" r="D11">
+        <v>69</v>
+      </c>
+      <c t="s" s="1" r="F11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12">
+      <c t="s" s="1" r="A12">
+        <v>71</v>
+      </c>
+      <c t="s" s="1" r="B12">
+        <v>72</v>
+      </c>
+      <c t="s" s="1" r="C12">
+        <v>73</v>
+      </c>
+      <c t="s" s="1" r="D12">
+        <v>74</v>
+      </c>
+      <c t="s" s="1" r="F12">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13">
+      <c t="s" s="1" r="A13">
+        <v>76</v>
+      </c>
+      <c t="s" s="1" r="B13">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="C13">
+        <v>78</v>
+      </c>
+      <c t="s" s="1" r="D13">
+        <v>79</v>
+      </c>
+      <c t="s" s="1" r="F13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14">
+      <c t="s" s="1" r="A14">
+        <v>81</v>
+      </c>
+      <c t="s" s="1" r="B14">
+        <v>82</v>
+      </c>
+      <c t="s" s="1" r="C14">
+        <v>83</v>
+      </c>
+      <c t="s" s="1" r="D14">
+        <v>84</v>
+      </c>
+      <c t="s" s="1" r="F14">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15">
+      <c t="s" s="1" r="A15">
+        <v>86</v>
+      </c>
+      <c t="s" s="1" r="B15">
+        <v>87</v>
+      </c>
+      <c t="s" s="1" r="C15">
+        <v>88</v>
+      </c>
+      <c t="s" s="1" r="D15">
+        <v>89</v>
+      </c>
+      <c t="s" s="5" r="E15">
+        <v>90</v>
+      </c>
+      <c t="s" s="1" r="F15">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" customWidth="1" max="1" width="22.86"/>
     <col min="2" customWidth="1" max="2" width="21.14"/>
@@ -1258,10 +1435,10 @@
   <sheetData>
     <row customHeight="1" r="1" ht="14.25">
       <c t="s" s="1" r="A1">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c t="s" s="1" r="B1">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c s="3" r="C1"/>
       <c s="3" r="D1"/>
@@ -1276,10 +1453,10 @@
     </row>
     <row customHeight="1" r="2" ht="14.25">
       <c t="s" s="1" r="A2">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c t="s" s="1" r="B2">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c s="3" r="C2"/>
       <c s="3" r="D2"/>

</xml_diff>